<commit_message>
Completed 3rd subfolder of stacks
</commit_message>
<xml_diff>
--- a/DS Striver Sheet latest.xlsx
+++ b/DS Striver Sheet latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Notes\DSA\A2Z\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Notes\DSA\A2Z Striver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B24C2A-D689-4D0E-B3CB-5811C9A13585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F3782-D2C0-43C3-B845-3E36E1249909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="822" firstSheet="19" activeTab="25" xr2:uid="{F77BB47A-5C51-4208-A74B-09BD4705F65C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="822" firstSheet="25" activeTab="28" xr2:uid="{F77BB47A-5C51-4208-A74B-09BD4705F65C}"/>
   </bookViews>
   <sheets>
     <sheet name="Learn The Basics" sheetId="2" r:id="rId1"/>
@@ -39,6 +39,12 @@
     <sheet name="Interview Prob of Bit Mani." sheetId="25" r:id="rId24"/>
     <sheet name="Advanced Maths" sheetId="26" r:id="rId25"/>
     <sheet name="Learning Stacks N Queues" sheetId="22" r:id="rId26"/>
+    <sheet name="Prefix, Infix and Postfix" sheetId="27" r:id="rId27"/>
+    <sheet name="Monotonic Stack" sheetId="28" r:id="rId28"/>
+    <sheet name="Implementation Problems" sheetId="32" r:id="rId29"/>
+    <sheet name="Graph Learning" sheetId="29" r:id="rId30"/>
+    <sheet name="Problems on BFS &amp; DFS" sheetId="30" r:id="rId31"/>
+    <sheet name="Topo Sort and Problems" sheetId="31" r:id="rId32"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="295">
   <si>
     <t>S.no</t>
   </si>
@@ -782,6 +788,159 @@
   </si>
   <si>
     <t>Implement Min Stack</t>
+  </si>
+  <si>
+    <t>Infix to Postfix Conversion using Stack</t>
+  </si>
+  <si>
+    <t>Prefix to Infix Conversion</t>
+  </si>
+  <si>
+    <t>Prefix to Postfix Conversion</t>
+  </si>
+  <si>
+    <t>Postfix to Prefix Conversion</t>
+  </si>
+  <si>
+    <t>Postfix to Infix</t>
+  </si>
+  <si>
+    <t>Convert Infix To Prefix Notation</t>
+  </si>
+  <si>
+    <t>Next Greater Element</t>
+  </si>
+  <si>
+    <t>Next Greater Element 2</t>
+  </si>
+  <si>
+    <t>Next Smaller Element</t>
+  </si>
+  <si>
+    <t>Number of NGEs to the right</t>
+  </si>
+  <si>
+    <t>Trapping Rainwater</t>
+  </si>
+  <si>
+    <t>Sum of subarray minimum</t>
+  </si>
+  <si>
+    <t>Asteroid Collision</t>
+  </si>
+  <si>
+    <t>Sum of subarray ranges</t>
+  </si>
+  <si>
+    <t>Remove k Digits</t>
+  </si>
+  <si>
+    <t>Largest rectangle in a histogram</t>
+  </si>
+  <si>
+    <t>Maximal Rectangles</t>
+  </si>
+  <si>
+    <t>IB</t>
+  </si>
+  <si>
+    <t>Graph and Types</t>
+  </si>
+  <si>
+    <t>Graph Representation | C++</t>
+  </si>
+  <si>
+    <t>Graph Representation | Java</t>
+  </si>
+  <si>
+    <t>Connected Components | Logic Explanation</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>Number of provinces (leetcode)</t>
+  </si>
+  <si>
+    <t>Connected Components Problem in Matrix</t>
+  </si>
+  <si>
+    <t>Rotten Oranges</t>
+  </si>
+  <si>
+    <t>Flood fill</t>
+  </si>
+  <si>
+    <t>Cycle Detection in unirected Graph (bfs)</t>
+  </si>
+  <si>
+    <t>Cycle Detection in undirected Graph (dfs)</t>
+  </si>
+  <si>
+    <t>0/1 Matrix (Bfs Problem)</t>
+  </si>
+  <si>
+    <t>Surrounded Regions (dfs)</t>
+  </si>
+  <si>
+    <t>Number of Enclaves [flood fill implementation - multisource]</t>
+  </si>
+  <si>
+    <t>Word ladder - 1</t>
+  </si>
+  <si>
+    <t>Word ladder - 2</t>
+  </si>
+  <si>
+    <t>Number of Distinct Islands [dfs multisource]</t>
+  </si>
+  <si>
+    <t>Bipartite Graph (DFS)</t>
+  </si>
+  <si>
+    <t>Cycle Detection in Directed Graph (DFS)</t>
+  </si>
+  <si>
+    <t>Topo Sort</t>
+  </si>
+  <si>
+    <t>Kahn's Algorithm</t>
+  </si>
+  <si>
+    <t>Cycle Detection in Directed Graph (BFS)</t>
+  </si>
+  <si>
+    <t>Course Schedule - I</t>
+  </si>
+  <si>
+    <t>Course Schedule - II</t>
+  </si>
+  <si>
+    <t>Find eventual safe states</t>
+  </si>
+  <si>
+    <t>Alien dictionary</t>
+  </si>
+  <si>
+    <t>hoi</t>
+  </si>
+  <si>
+    <t>Sliding Window maximum</t>
+  </si>
+  <si>
+    <t>Stock span problem</t>
+  </si>
+  <si>
+    <t>The Celebrity Problem</t>
+  </si>
+  <si>
+    <t>LRU cache (IMPORTANT)</t>
+  </si>
+  <si>
+    <t>LFU cache</t>
   </si>
 </sst>
 </file>
@@ -1247,9 +1406,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1287,7 +1446,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1393,7 +1552,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1535,7 +1694,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1545,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD591641-4CBC-4554-9BB6-E97658E90AE6}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView zoomScale="152" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="152" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -5084,7 +5243,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5764,8 +5923,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6239,7 +6398,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6434,8 +6593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23911FB-DA38-469F-957E-C59380A9F3FB}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6712,6 +6871,803 @@
     <hyperlink ref="B9" r:id="rId16" display="https://takeuforward.org/data-structure/implement-min-stack-o2n-and-on-space-complexity/" xr:uid="{3DD06D4B-9B9F-4C69-A2F9-D93610061364}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B58564A-4BC1-4835-9E4B-FD68E0EEC289}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9">
+        <v>45457</v>
+      </c>
+      <c r="J2" s="9">
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9">
+        <v>45457</v>
+      </c>
+      <c r="J3" s="9">
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="9">
+        <v>45457</v>
+      </c>
+      <c r="J4" s="9">
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="9">
+        <v>45457</v>
+      </c>
+      <c r="J5" s="9">
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="9">
+        <v>45457</v>
+      </c>
+      <c r="J6" s="9">
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="9">
+        <v>45457</v>
+      </c>
+      <c r="J7" s="9">
+        <v>45457</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D70BEBD6-1B33-4119-93FC-BBD353FBC9CD}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{363982EC-CAB3-4426-94F6-C5EFF50CF02C}"/>
+    <hyperlink ref="E4" r:id="rId3" display="LC" xr:uid="{111ED34A-5670-444C-BD68-3EA556B68E6C}"/>
+    <hyperlink ref="E6" r:id="rId4" display="LC" xr:uid="{34BA7CF5-9DCE-4E56-BAC1-F76BE73A8C9B}"/>
+    <hyperlink ref="E5" r:id="rId5" display="LC" xr:uid="{F2DE7BD3-8011-4B21-9960-6A8D2C0503B3}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{8B4B6EEA-55A5-4DAD-9566-0A42F8C2F4C0}"/>
+    <hyperlink ref="B2" r:id="rId7" display="https://takeuforward.org/data-structure/infix-to-postfix/" xr:uid="{7EED2D3B-BC49-4483-9AB6-B1A2A9BAE0FA}"/>
+    <hyperlink ref="B3" r:id="rId8" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{39E6A1A9-BC04-49A8-A6B0-FFEF2274618B}"/>
+    <hyperlink ref="B4" r:id="rId9" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{3C98A4EF-B9F1-4C00-BA85-93D1412C02DD}"/>
+    <hyperlink ref="B5" r:id="rId10" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{59B2E51C-C9A8-4452-A865-69C7D05828E8}"/>
+    <hyperlink ref="B6" r:id="rId11" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{7E2849EE-27E1-4460-8DB2-97F2A150FB18}"/>
+    <hyperlink ref="B7" r:id="rId12" display="https://takeuforward.org/data-structure/infix-to-prefix/" xr:uid="{F487344C-89AA-42E8-8D0C-4444FA235069}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF61052-3DB8-4D76-9486-E6BDD729D5D2}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9">
+        <v>45458</v>
+      </c>
+      <c r="J2" s="9">
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9">
+        <v>45458</v>
+      </c>
+      <c r="J3" s="9">
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="9">
+        <v>45458</v>
+      </c>
+      <c r="J4" s="9">
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="9">
+        <v>45458</v>
+      </c>
+      <c r="J5" s="9">
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="9">
+        <v>45458</v>
+      </c>
+      <c r="J6" s="9">
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="9">
+        <v>45537</v>
+      </c>
+      <c r="J7" s="9">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="9">
+        <v>45537</v>
+      </c>
+      <c r="J8" s="9">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="9">
+        <v>45537</v>
+      </c>
+      <c r="J9" s="9">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9">
+        <v>45538</v>
+      </c>
+      <c r="J10" s="9">
+        <v>45538</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="9">
+        <v>45538</v>
+      </c>
+      <c r="J11" s="9">
+        <v>45538</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="9">
+        <v>45538</v>
+      </c>
+      <c r="J12" s="9">
+        <v>45538</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="CN" xr:uid="{72EEA73E-5674-4092-90CA-BC49E535309F}"/>
+    <hyperlink ref="E3" r:id="rId2" display="GFG" xr:uid="{B7BFD453-49FB-437F-85DD-0C6810D6B22F}"/>
+    <hyperlink ref="E4" r:id="rId3" display="LC" xr:uid="{376B2C43-62C1-46F6-B47B-CD8BC4ED27BE}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{F1074F14-497B-4A34-8BFF-1920F74E7CFF}"/>
+    <hyperlink ref="E5" r:id="rId5" display="LC" xr:uid="{0EED8E4E-3DD6-40A4-BB71-F8CE5AB26E3D}"/>
+    <hyperlink ref="E7" r:id="rId6" display="GFG" xr:uid="{D7ED4E5B-AE7F-465E-B451-4E1EA8C63A43}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{EE5C90E0-5F64-4A1A-A823-9A48D9C20CF4}"/>
+    <hyperlink ref="E10" r:id="rId8" display="CN" xr:uid="{548189B9-1CFF-4F58-8E0F-4941130FE4DB}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{FEA2694B-6544-4C49-8420-E28CC89258CB}"/>
+    <hyperlink ref="E12" r:id="rId10" display="CN" xr:uid="{9BE3B8FC-B094-4FC0-85BA-79984C54105D}"/>
+    <hyperlink ref="E9" r:id="rId11" display="CN" xr:uid="{E968A123-CA13-44BE-8234-372AD2472DBF}"/>
+    <hyperlink ref="B2" r:id="rId12" display="https://takeuforward.org/data-structure/next-greater-element-using-stack/" xr:uid="{90ED4A44-91ED-4E42-906B-5FCFAB16D3AC}"/>
+    <hyperlink ref="B3" r:id="rId13" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{89D2474D-A2AF-4A69-96FF-023B612EB975}"/>
+    <hyperlink ref="B6" r:id="rId14" display="https://takeuforward.org/data-structure/trapping-rainwater/" xr:uid="{3E6900F8-0056-40CB-9199-3E1A95862791}"/>
+    <hyperlink ref="B7" r:id="rId15" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{7D934CAC-E26F-4C93-A502-1EA9516B23B2}"/>
+    <hyperlink ref="B8" r:id="rId16" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{B973C918-8FDD-4ED6-8A2F-C5EDA43A9A0E}"/>
+    <hyperlink ref="B9" r:id="rId17" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{A2DFAA31-F9C0-45C7-BE83-415B10A22481}"/>
+    <hyperlink ref="B10" r:id="rId18" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{122B1DCF-4B71-4184-A7DD-42E4B409BECF}"/>
+    <hyperlink ref="B11" r:id="rId19" display="https://takeuforward.org/data-structure/area-of-largest-rectangle-in-histogram/" xr:uid="{AB1BE4D5-FF17-4BBC-84AB-190C4BB9E77A}"/>
+    <hyperlink ref="B12" r:id="rId20" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{30C7635E-F9B5-4B06-95B3-92D8E7194102}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7EE952F-A14D-4531-9490-1B572FA58BDA}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J2" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J3" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J4" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J5" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J6" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="GFG" xr:uid="{7256A0B0-C8C7-4015-9D3B-01488908F654}"/>
+    <hyperlink ref="E3" r:id="rId2" display="GFG" xr:uid="{413B7D9A-C116-4746-8288-F3AAD01296D7}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{AB81EB66-8F88-40A3-BB1D-CA1CDADF6ADE}"/>
+    <hyperlink ref="E6" r:id="rId4" display="GFG" xr:uid="{C379F9D1-D202-4739-BA42-2BCE53B946D3}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{26E16C72-5FFB-4EF0-852B-8434187EB296}"/>
+    <hyperlink ref="B2" r:id="rId6" display="https://takeuforward.org/data-structure/sliding-window-maximum/" xr:uid="{0928A63E-FBF0-4EE9-97EC-0A238C3955AF}"/>
+    <hyperlink ref="B3" r:id="rId7" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{670A6096-0655-4E36-9D58-797B51258EF2}"/>
+    <hyperlink ref="B4" r:id="rId8" display="https://takeuforward.org/strivers-a2z-dsa-course/strivers-a2z-dsa-course-sheet-2/" xr:uid="{1E45011E-1FCA-4437-BE93-3AB9B9E9B27E}"/>
+    <hyperlink ref="B5" r:id="rId9" display="https://takeuforward.org/data-structure/implement-lru-cache/" xr:uid="{520B1698-FFA9-4615-956A-5EE82DD1AA67}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -7021,11 +7977,936 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAC01FA-66E1-4A6C-827D-21A8F0025CA6}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J2" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J3" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J4" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J5" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J6" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="9">
+        <v>45529</v>
+      </c>
+      <c r="J7" s="9">
+        <v>45529</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C56D7C2F-8A62-4015-8393-000D7A59B0EC}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{C4C97B16-E972-4862-A679-207EBB36A0BE}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{FC11F080-4E42-4A58-B2FE-45C53EA26D8B}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{1C9C5F02-6D34-4C07-B64B-E17311F82AFF}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{AC87B1D5-6480-4131-9E38-9C70377CCD0C}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{E041ED07-DB16-4907-B9F7-CBC395F9CFC4}"/>
+    <hyperlink ref="B2" r:id="rId7" display="https://takeuforward.org/graph/introduction-to-graph/" xr:uid="{2EB3A39F-E337-49E6-B8BE-5710768761D7}"/>
+    <hyperlink ref="B3" r:id="rId8" display="https://takeuforward.org/graph/graph-representation-in-c/" xr:uid="{2E61F752-68F9-47B4-A407-80C9FDFC50D8}"/>
+    <hyperlink ref="B5" r:id="rId9" display="https://takeuforward.org/graph/connected-components-in-graphs/" xr:uid="{AC51123D-DEDD-471D-BB41-28B8E0EBAD49}"/>
+    <hyperlink ref="B6" r:id="rId10" display="https://takeuforward.org/graph/breadth-first-search-bfs-level-order-traversal/" xr:uid="{2E6E1FDA-6273-4D04-AFC3-85033A30ACD0}"/>
+    <hyperlink ref="B7" r:id="rId11" display="https://takeuforward.org/data-structure/depth-first-search-dfs/" xr:uid="{0B96592A-B6AB-4F40-8844-7F9F50FED3A6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259372A3-4B37-4936-8BE2-E142E5A1D7ED}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9">
+        <v>45531</v>
+      </c>
+      <c r="J2" s="9">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9">
+        <v>45531</v>
+      </c>
+      <c r="J3" s="9">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="9">
+        <v>45531</v>
+      </c>
+      <c r="J4" s="9">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="9">
+        <v>45531</v>
+      </c>
+      <c r="J5" s="9">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="9">
+        <v>45531</v>
+      </c>
+      <c r="J6" s="9">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="9">
+        <v>45531</v>
+      </c>
+      <c r="J7" s="9">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="9">
+        <v>45531</v>
+      </c>
+      <c r="J8" s="9">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="9">
+        <v>45532</v>
+      </c>
+      <c r="J9" s="9">
+        <v>45532</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9">
+        <v>45532</v>
+      </c>
+      <c r="J10" s="9">
+        <v>45532</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="9">
+        <v>45472</v>
+      </c>
+      <c r="J11" s="9">
+        <v>45472</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="9">
+        <v>45472</v>
+      </c>
+      <c r="J12" s="9">
+        <v>45472</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="9">
+        <v>45533</v>
+      </c>
+      <c r="J13" s="9">
+        <v>45533</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="9">
+        <v>45533</v>
+      </c>
+      <c r="J14" s="9">
+        <v>45533</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="9">
+        <v>45533</v>
+      </c>
+      <c r="J15" s="9">
+        <v>45533</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="CN" xr:uid="{1EEC696F-1525-42E8-895C-6E2AD3422E52}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{6B38B67A-7238-466E-AFFC-E43365AE5857}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{E178C4E9-FA7A-43DC-ACF8-4C4193B276FB}"/>
+    <hyperlink ref="E6" r:id="rId4" display="LC" xr:uid="{9273CE84-23D8-4FCF-9511-D00C8FB4D26E}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{D0384D78-8892-4D23-9F8F-9480E5AD380E}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{503026FD-7CD3-4F8B-A111-76794A6CE99C}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{54E0B796-49D0-4212-A714-8F4D6751A4E8}"/>
+    <hyperlink ref="E10" r:id="rId8" display="CN" xr:uid="{2B38D4C9-249E-4624-9D87-F557FAC45782}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{019B415E-EAE1-4F2C-AFC1-1F20079AEA18}"/>
+    <hyperlink ref="E12" r:id="rId10" display="CN" xr:uid="{0949543A-83E7-4E87-8701-7A336B615BB9}"/>
+    <hyperlink ref="E9" r:id="rId11" display="CN" xr:uid="{842D174B-8582-4656-9815-48E6C7FB30A1}"/>
+    <hyperlink ref="E13" r:id="rId12" display="CN" xr:uid="{E4E00F10-39BD-4E09-B6E7-9CE8A6ACE4D1}"/>
+    <hyperlink ref="E14" r:id="rId13" display="CN" xr:uid="{5E954CC4-D250-4397-8A74-9BBB7B109B88}"/>
+    <hyperlink ref="E15" r:id="rId14" display="CN" xr:uid="{56A78A83-EFC6-43B9-8A68-E773F81816CA}"/>
+    <hyperlink ref="B2" r:id="rId15" display="https://takeuforward.org/data-structure/number-of-provinces/" xr:uid="{19985B49-EF69-4342-8DDD-3ACAAF4692F5}"/>
+    <hyperlink ref="B4" r:id="rId16" display="https://takeuforward.org/data-structure/rotten-oranges-min-time-to-rot-all-oranges-bfs/" xr:uid="{C977C7EA-ECD1-4182-BA76-8740EAB6F6A2}"/>
+    <hyperlink ref="B5" r:id="rId17" display="https://takeuforward.org/graph/flood-fill-algorithm-graphs/" xr:uid="{3A3C68A2-E0AB-47A4-B80B-56B04B05E755}"/>
+    <hyperlink ref="B6" r:id="rId18" display="https://takeuforward.org/data-structure/detect-cycle-in-an-undirected-graph-using-bfs/" xr:uid="{0D501CE9-1E70-42EF-9CA5-A1FBA7AEC7DC}"/>
+    <hyperlink ref="B7" r:id="rId19" display="https://takeuforward.org/data-structure/detect-cycle-in-an-undirected-graph-using-dfs/" xr:uid="{E76FE3E0-3113-41E5-8C85-0878C6493CE8}"/>
+    <hyperlink ref="B8" r:id="rId20" display="https://takeuforward.org/graph/distance-of-nearest-cell-having-1/" xr:uid="{F0D795D2-4860-47AA-8145-E1A453567EBC}"/>
+    <hyperlink ref="B9" r:id="rId21" display="https://takeuforward.org/graph/surrounded-regions-replace-os-with-xs/" xr:uid="{8124E3A9-CF21-4CFE-B1B5-2C856D0B3960}"/>
+    <hyperlink ref="B10" r:id="rId22" display="https://takeuforward.org/graph/number-of-enclaves/" xr:uid="{A39716A2-508B-4D40-B97E-EE3F7E09BD08}"/>
+    <hyperlink ref="B11" r:id="rId23" display="https://takeuforward.org/graph/word-ladder-i-g-29/" xr:uid="{F7CBB8CE-0186-496F-9CA7-A71B20E3DEF4}"/>
+    <hyperlink ref="B12" r:id="rId24" display="https://takeuforward.org/graph/g-30-word-ladder-ii/" xr:uid="{5BD65F32-3B7A-49EB-A896-68C4E305D56A}"/>
+    <hyperlink ref="B13" r:id="rId25" display="https://takeuforward.org/data-structure/number-of-islands/" xr:uid="{9D045954-0F57-4B24-8F72-362CAC0A666B}"/>
+    <hyperlink ref="B14" r:id="rId26" display="https://takeuforward.org/graph/bipartite-graph-dfs-implementation/" xr:uid="{995BEF93-5819-4D9D-9F95-FD193DA91F96}"/>
+    <hyperlink ref="B15" r:id="rId27" display="https://takeuforward.org/data-structure/detect-cycle-in-a-directed-graph-using-dfs-g-19/" xr:uid="{351AF6C7-70C5-44A5-882C-88487FD6BBD8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA849ED-CADD-4523-A985-B923048DCC68}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView zoomScale="178" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9">
+        <v>45470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9">
+        <v>45470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9">
+        <v>45470</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9">
+        <v>45463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9">
+        <v>45463</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="9">
+        <v>45533</v>
+      </c>
+      <c r="J7" s="9">
+        <v>45533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9">
+        <v>45464</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{604AFD5A-DA73-40E7-BA7F-6363EDE75E5D}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{C161711A-EE0D-453D-B0DD-92A72E21432C}"/>
+    <hyperlink ref="E4" r:id="rId3" display="LC" xr:uid="{9FA42A11-71E4-4676-8DF9-5CCE1C208F9B}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{5A5C0D54-3434-4471-9294-AA67DC6654AD}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{12814CEA-497F-418F-B0CB-0AE6E8D22EB2}"/>
+    <hyperlink ref="E7" r:id="rId6" display="GFG" xr:uid="{984BB8F1-CA01-4B07-9529-59557F4D3D34}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{E0426C76-090D-4C09-9A4D-937FD4619EF4}"/>
+    <hyperlink ref="B2" r:id="rId8" display="https://takeuforward.org/data-structure/topological-sort-algorithm-dfs-g-21/" xr:uid="{11200B57-A189-4DA0-B121-D1723A512914}"/>
+    <hyperlink ref="B3" r:id="rId9" display="https://takeuforward.org/data-structure/kahns-algorithm-topological-sort-algorithm-bfs-g-22/" xr:uid="{113A0934-A44C-42B3-B61A-A75AD3AB440F}"/>
+    <hyperlink ref="B5" r:id="rId10" display="https://takeuforward.org/data-structure/course-schedule-i-and-ii-pre-requisite-tasks-topological-sort-g-24/" xr:uid="{0CA046E5-5816-4C4E-92EB-0D3977FB2981}"/>
+    <hyperlink ref="B6" r:id="rId11" display="https://takeuforward.org/data-structure/course-schedule-i-and-ii-pre-requisite-tasks-topological-sort-g-24/" xr:uid="{1545D9BB-8FE4-4BC1-800E-B8F3105FFA2E}"/>
+    <hyperlink ref="B7" r:id="rId12" display="https://takeuforward.org/data-structure/find-eventual-safe-states-bfs-topological-sort-g-25/" xr:uid="{E8A0006F-A7FB-4904-97D0-4E49DE6FF35E}"/>
+    <hyperlink ref="B8" r:id="rId13" display="https://takeuforward.org/data-structure/alien-dictionary-topological-sort-g-26/" xr:uid="{0F0E7102-26E1-401B-9F7C-CAAF83A7AF2E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AB9957-EC6C-44AB-93EC-185AA421BD58}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="154" workbookViewId="0">
+    <sheetView zoomScale="74" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -8029,7 +9910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2BF9F3-8D83-498D-82C1-BA001B66B011}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="AH1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>